<commit_message>
ended xls files of tests
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_01_hold2.xlsx
+++ b/results_analysis/spark_cervicalCancer_01_hold2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24247D7E-9973-4A78-B47B-BC21C46B84DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45887021-C104-46C6-A4F8-21C6247C48D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -614,21 +614,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -647,13 +632,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -666,9 +645,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -695,6 +671,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,6 +693,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,19 +999,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1074,7 +1059,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="44">
         <v>0.42578397212543601</v>
       </c>
       <c r="E5" s="12">
@@ -1095,7 +1080,7 @@
       <c r="J5" s="12">
         <v>0.36411149825784</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="45">
         <v>0.37979094076655101</v>
       </c>
     </row>
@@ -1104,7 +1089,7 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="46">
         <v>0.39686411149825801</v>
       </c>
       <c r="E6" s="13">
@@ -1137,7 +1122,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="46">
         <v>0.39721254355400698</v>
       </c>
       <c r="E7" s="13">
@@ -1168,7 +1153,7 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="47">
         <v>0.43222996515679402</v>
       </c>
       <c r="E8" s="14">
@@ -1189,7 +1174,7 @@
       <c r="J8" s="14">
         <v>0.41411149825783999</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="48">
         <v>0.40191637630662003</v>
       </c>
     </row>
@@ -1203,28 +1188,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="49">
         <v>0.39407665505226502</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="50">
         <v>0.39773519163763099</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="50">
         <v>0.37282229965156799</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="50">
         <v>0.40975609756097597</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="50">
         <v>0.39285714285714302</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="50">
         <v>0.15331010452961699</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="50">
         <v>0.36724738675958202</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="51">
         <v>0.39285714285714302</v>
       </c>
     </row>
@@ -1233,7 +1218,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="46">
         <v>0.412020905923345</v>
       </c>
       <c r="E10" s="13">
@@ -1266,7 +1251,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="46">
         <v>0.39494773519163801</v>
       </c>
       <c r="E11" s="13">
@@ -1297,7 +1282,7 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="47">
         <v>0.39581881533100999</v>
       </c>
       <c r="E12" s="14">
@@ -1318,7 +1303,7 @@
       <c r="J12" s="14">
         <v>0.40644599303135898</v>
       </c>
-      <c r="K12" s="56">
+      <c r="K12" s="48">
         <v>0.43519163763066199</v>
       </c>
     </row>
@@ -1332,28 +1317,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="49">
         <v>0.395644599303136</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="50">
         <v>0.40017421602787501</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="50">
         <v>0.38397212543553999</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="50">
         <v>0.38310104529616701</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="50">
         <v>0.36829268292682898</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="50">
         <v>0.38693379790940802</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="50">
         <v>0.37038327526132397</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="51">
         <v>0.39320557491289199</v>
       </c>
     </row>
@@ -1362,7 +1347,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="46">
         <v>0.42404181184668999</v>
       </c>
       <c r="E14" s="13">
@@ -1395,7 +1380,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="46">
         <v>0.34198606271776999</v>
       </c>
       <c r="E15" s="13">
@@ -1426,7 +1411,7 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="47">
         <v>0.333275261324042</v>
       </c>
       <c r="E16" s="14">
@@ -1447,7 +1432,7 @@
       <c r="J16" s="14">
         <v>0.23118466898954701</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="48">
         <v>0.19668989547038301</v>
       </c>
     </row>
@@ -1461,28 +1446,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="49">
         <v>0.463240418118467</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="50">
         <v>0.46010452961672499</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="50">
         <v>0.40331010452961702</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="50">
         <v>0.43658536585365898</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="50">
         <v>0.42212543554006998</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="50">
         <v>0.36202090592334502</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="50">
         <v>0.36986062717770002</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K17" s="51">
         <v>0.44529616724738702</v>
       </c>
     </row>
@@ -1491,7 +1476,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="46">
         <v>0.48780487804878098</v>
       </c>
       <c r="E18" s="13">
@@ -1524,7 +1509,7 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="46">
         <v>0.398257839721254</v>
       </c>
       <c r="E19" s="13">
@@ -1555,7 +1540,7 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="47">
         <v>0.44477351916376301</v>
       </c>
       <c r="E20" s="14">
@@ -1576,7 +1561,7 @@
       <c r="J20" s="14">
         <v>0.41114982578397202</v>
       </c>
-      <c r="K20" s="56">
+      <c r="K20" s="48">
         <v>0.40452961672473903</v>
       </c>
     </row>
@@ -1924,7 +1909,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,19 +1920,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2004,7 +1989,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="44">
         <v>0.373201569155796</v>
       </c>
       <c r="E5" s="12">
@@ -2025,7 +2010,7 @@
       <c r="J5" s="12">
         <v>0.33301410915232199</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="45">
         <v>0.33256548162963301</v>
       </c>
     </row>
@@ -2035,7 +2020,7 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="46">
         <v>0.33014224972566197</v>
       </c>
       <c r="E6" s="13">
@@ -2068,7 +2053,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="46">
         <v>0.31811329709653802</v>
       </c>
       <c r="E7" s="13">
@@ -2099,7 +2084,7 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="47">
         <v>0.37691846913705002</v>
       </c>
       <c r="E8" s="14">
@@ -2120,7 +2105,7 @@
       <c r="J8" s="14">
         <v>0.36109529586667299</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="48">
         <v>0.33528435412030599</v>
       </c>
     </row>
@@ -2134,28 +2119,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="49">
         <v>0.35215709416256702</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="50">
         <v>0.32160556765619203</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="50">
         <v>0.32799810597364798</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="50">
         <v>0.35338898193083101</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="50">
         <v>0.32364314884547501</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="50">
         <v>0</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="50">
         <v>0.32759405456213497</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="51">
         <v>0.36282915900350199</v>
       </c>
     </row>
@@ -2165,7 +2150,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="46">
         <v>0.33466113792874602</v>
       </c>
       <c r="E10" s="13">
@@ -2198,7 +2183,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="46">
         <v>0.32212426492877499</v>
       </c>
       <c r="E11" s="13">
@@ -2229,7 +2214,7 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="47">
         <v>0.37682414097359301</v>
       </c>
       <c r="E12" s="14">
@@ -2250,7 +2235,7 @@
       <c r="J12" s="14">
         <v>0.38074118273512803</v>
       </c>
-      <c r="K12" s="56">
+      <c r="K12" s="48">
         <v>0.42869453500190202</v>
       </c>
     </row>
@@ -2264,28 +2249,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="49">
         <v>0.33034570452662199</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="50">
         <v>0.32280504766857998</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="50">
         <v>0.31181149892057702</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="50">
         <v>0.32527116129531602</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="50">
         <v>0.31445713260503</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="50">
         <v>0.32671874254313299</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="50">
         <v>0.34965101234157703</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="51">
         <v>0.32515963600125902</v>
       </c>
     </row>
@@ -2295,7 +2280,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="46">
         <v>0.35704245185970601</v>
       </c>
       <c r="E14" s="13">
@@ -2328,7 +2313,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="46">
         <v>0.27681489008084997</v>
       </c>
       <c r="E15" s="13">
@@ -2359,7 +2344,7 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="47">
         <v>0.26186993009514198</v>
       </c>
       <c r="E16" s="14">
@@ -2380,7 +2365,7 @@
       <c r="J16" s="14">
         <v>0.222237996442092</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="48">
         <v>0.30496302706837197</v>
       </c>
     </row>
@@ -2394,28 +2379,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="49">
         <v>0.38392762996065399</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="50">
         <v>0.39149925367019001</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="50">
         <v>0.30925267167572001</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="50">
         <v>0.37020262497060702</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="50">
         <v>0.36611606867651603</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="50">
         <v>0.30008886925076</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="50">
         <v>0.34437902759456002</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K17" s="51">
         <v>0.40065052739708901</v>
       </c>
     </row>
@@ -2425,7 +2410,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="46">
         <v>0.44520639519432498</v>
       </c>
       <c r="E18" s="13">
@@ -2458,7 +2443,7 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="46">
         <v>0.31990643520175499</v>
       </c>
       <c r="E19" s="13">
@@ -2489,7 +2474,7 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="47">
         <v>0.38628657844787201</v>
       </c>
       <c r="E20" s="14">
@@ -2510,7 +2495,7 @@
       <c r="J20" s="14">
         <v>0.42111665188502301</v>
       </c>
-      <c r="K20" s="56">
+      <c r="K20" s="48">
         <v>0.36536116181506401</v>
       </c>
     </row>
@@ -2527,7 +2512,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,19 +2523,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2607,7 +2592,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="44">
         <v>0.51608439282831597</v>
       </c>
       <c r="E5" s="12">
@@ -2628,7 +2613,7 @@
       <c r="J5" s="12">
         <v>0.53445928129354603</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="45">
         <v>0.491968228098706</v>
       </c>
     </row>
@@ -2638,7 +2623,7 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="46">
         <v>0.55674521887026795</v>
       </c>
       <c r="E6" s="13">
@@ -2671,7 +2656,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="46">
         <v>0.49741073283042397</v>
       </c>
       <c r="E7" s="13">
@@ -2702,7 +2687,7 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="47">
         <v>0.52956055450344197</v>
       </c>
       <c r="E8" s="14">
@@ -2723,7 +2708,7 @@
       <c r="J8" s="14">
         <v>0.53665048998656495</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="48">
         <v>0.50455964779416396</v>
       </c>
     </row>
@@ -2737,28 +2722,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="49">
         <v>0.51093097748043304</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="50">
         <v>0.47564349588072902</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="50">
         <v>0.51901252474919402</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="50">
         <v>0.52270207674952895</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="50">
         <v>0.45385667292447202</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="50">
         <v>5.8567471309853597E-2</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="50">
         <v>0.41624190934936001</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="51">
         <v>0.50213385521349696</v>
       </c>
     </row>
@@ -2768,7 +2753,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="46">
         <v>0.50062350990232796</v>
       </c>
       <c r="E10" s="13">
@@ -2801,7 +2786,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="46">
         <v>0.53246694795815697</v>
       </c>
       <c r="E11" s="13">
@@ -2832,7 +2817,7 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="47">
         <v>0.44038347379175602</v>
       </c>
       <c r="E12" s="14">
@@ -2853,7 +2838,7 @@
       <c r="J12" s="14">
         <v>0.56452453626433097</v>
       </c>
-      <c r="K12" s="56">
+      <c r="K12" s="48">
         <v>0.56938536082184699</v>
       </c>
     </row>
@@ -2867,28 +2852,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="49">
         <v>0.484441052646012</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="50">
         <v>0.51174221770512696</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="50">
         <v>0.46517408818390199</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="50">
         <v>0.496926987630112</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="50">
         <v>0.48780864448045902</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="50">
         <v>0.49839927744106399</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="50">
         <v>0.525322058146516</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="51">
         <v>0.52015982043365006</v>
       </c>
     </row>
@@ -2898,7 +2883,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="46">
         <v>0.53948860005517996</v>
       </c>
       <c r="E14" s="13">
@@ -2931,7 +2916,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="46">
         <v>0.42364372840417902</v>
       </c>
       <c r="E15" s="13">
@@ -2962,7 +2947,7 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="47">
         <v>0.44147173653302402</v>
       </c>
       <c r="E16" s="14">
@@ -2983,7 +2968,7 @@
       <c r="J16" s="14">
         <v>0.38551937775735501</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="48">
         <v>0.43834636411635702</v>
       </c>
     </row>
@@ -2997,28 +2982,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="49">
         <v>0.58031883270586604</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="50">
         <v>0.578285854368778</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="50">
         <v>0.51435304953721706</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="50">
         <v>0.52628465438572702</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="50">
         <v>0.52728093176621005</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="50">
         <v>0.48980051174077899</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="50">
         <v>0.50147444504241401</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K17" s="51">
         <v>0.56714453110808205</v>
       </c>
     </row>
@@ -3028,7 +3013,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="46">
         <v>0.60741056055460196</v>
       </c>
       <c r="E18" s="13">
@@ -3061,7 +3046,7 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="46">
         <v>0.46313943580233302</v>
       </c>
       <c r="E19" s="13">
@@ -3092,7 +3077,7 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="47">
         <v>0.49681726398943299</v>
       </c>
       <c r="E20" s="14">
@@ -3113,7 +3098,7 @@
       <c r="J20" s="14">
         <v>0.58926530692106804</v>
       </c>
-      <c r="K20" s="56">
+      <c r="K20" s="48">
         <v>0.543475009425053</v>
       </c>
     </row>
@@ -3130,7 +3115,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,19 +3133,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3900,7 +3885,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,19 +3903,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3978,7 +3963,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="44">
         <v>0.494773519163763</v>
       </c>
       <c r="E5" s="12">
@@ -3999,7 +3984,7 @@
       <c r="J5" s="12">
         <v>0.45644599303135902</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="45">
         <v>0.43031358885017401</v>
       </c>
     </row>
@@ -4008,7 +3993,7 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="46">
         <v>0.454703832752613</v>
       </c>
       <c r="E6" s="13">
@@ -4041,7 +4026,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="46">
         <v>0.43379790940766599</v>
       </c>
       <c r="E7" s="13">
@@ -4072,7 +4057,7 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="47">
         <v>0.47212543554007003</v>
       </c>
       <c r="E8" s="14">
@@ -4093,7 +4078,7 @@
       <c r="J8" s="14">
         <v>0.47386759581881499</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="48">
         <v>0.45993031358885</v>
       </c>
     </row>
@@ -4107,28 +4092,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="49">
         <v>0.45644599303135902</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="50">
         <v>0.449477351916376</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="50">
         <v>0.45121951219512202</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="50">
         <v>0.46167247386759602</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="50">
         <v>0.41811846689895499</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="50">
         <v>0.257839721254355</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="50">
         <v>0.439024390243902</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="51">
         <v>0.46515679442508701</v>
       </c>
     </row>
@@ -4137,7 +4122,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="46">
         <v>0.45818815331010498</v>
       </c>
       <c r="E10" s="13">
@@ -4170,7 +4155,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="46">
         <v>0.44250871080139398</v>
       </c>
       <c r="E11" s="13">
@@ -4201,7 +4186,7 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="47">
         <v>0.46864111498257799</v>
       </c>
       <c r="E12" s="14">
@@ -4222,7 +4207,7 @@
       <c r="J12" s="14">
         <v>0.489547038327526</v>
       </c>
-      <c r="K12" s="56">
+      <c r="K12" s="48">
         <v>0.52439024390243905</v>
       </c>
     </row>
@@ -4236,28 +4221,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="49">
         <v>0.444250871080139</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="50">
         <v>0.44599303135888502</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="50">
         <v>0.43205574912891997</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="50">
         <v>0.44773519163763098</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="50">
         <v>0.43379790940766599</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="50">
         <v>0.444250871080139</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="50">
         <v>0.46864111498257799</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="51">
         <v>0.44250871080139398</v>
       </c>
     </row>
@@ -4266,7 +4251,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="46">
         <v>0.46167247386759602</v>
       </c>
       <c r="E14" s="13">
@@ -4299,7 +4284,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="46">
         <v>0.398954703832753</v>
       </c>
       <c r="E15" s="13">
@@ -4330,7 +4315,7 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="47">
         <v>0.39547038327526102</v>
       </c>
       <c r="E16" s="14">
@@ -4351,7 +4336,7 @@
       <c r="J16" s="14">
         <v>0.36411149825784</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="48">
         <v>0.393728222996516</v>
       </c>
     </row>
@@ -4365,28 +4350,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="49">
         <v>0.49825783972125398</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="50">
         <v>0.49825783972125398</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="50">
         <v>0.43728222996515698</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="50">
         <v>0.48257839721254397</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="50">
         <v>0.48432055749128899</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="50">
         <v>0.43554006968641101</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="50">
         <v>0.45993031358885</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K17" s="51">
         <v>0.50696864111498297</v>
       </c>
     </row>
@@ -4395,7 +4380,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="46">
         <v>0.54355400696864098</v>
       </c>
       <c r="E18" s="13">
@@ -4428,7 +4413,7 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="46">
         <v>0.43031358885017401</v>
       </c>
       <c r="E19" s="13">
@@ -4459,7 +4444,7 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="47">
         <v>0.48606271777003501</v>
       </c>
       <c r="E20" s="14">
@@ -4480,7 +4465,7 @@
       <c r="J20" s="14">
         <v>0.52264808362369297</v>
       </c>
-      <c r="K20" s="56">
+      <c r="K20" s="48">
         <v>0.47909407665505199</v>
       </c>
     </row>
@@ -4828,7 +4813,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4846,19 +4831,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5598,7 +5583,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5616,19 +5601,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6368,7 +6353,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6386,19 +6371,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7138,7 +7123,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7156,19 +7141,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7908,7 +7893,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:P20"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7916,40 +7901,40 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7959,29 +7944,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="62" t="s">
+      <c r="L3" s="57"/>
+      <c r="M3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="62" t="s">
+      <c r="N3" s="57"/>
+      <c r="O3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="64"/>
+      <c r="P3" s="58"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -8043,43 +8028,43 @@
       <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="43">
         <v>3.90625E-3</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="33">
         <v>32</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="52">
         <v>3.90625E-3</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="33">
         <v>512</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="33">
         <v>2.6</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="33">
         <v>16</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="33">
         <v>16</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="33">
         <v>3</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="33">
         <v>32</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="52">
         <v>7.8125E-3</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="52">
         <v>3.125E-2</v>
       </c>
-      <c r="O5" s="38">
-        <v>1</v>
-      </c>
-      <c r="P5" s="39">
+      <c r="O5" s="33">
+        <v>1</v>
+      </c>
+      <c r="P5" s="34">
         <v>32</v>
       </c>
     </row>
@@ -8088,43 +8073,43 @@
       <c r="C6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="36">
         <v>512</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="29">
         <v>8</v>
       </c>
       <c r="F6" s="29">
         <v>1</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>128</v>
       </c>
       <c r="H6" s="29">
         <v>2</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>32</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="30">
         <v>0.5</v>
       </c>
       <c r="K6" s="19">
         <v>2</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="29">
         <v>4</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M6" s="13">
         <v>9.765625E-4</v>
       </c>
       <c r="N6" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="O6" s="19">
-        <v>1</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="O6" s="29">
+        <v>1</v>
+      </c>
+      <c r="P6" s="39">
         <v>16</v>
       </c>
     </row>
@@ -8136,13 +8121,13 @@
       <c r="C7" s="22">
         <v>1</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="36">
         <v>64</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="29">
         <v>16</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="29">
         <v>4</v>
       </c>
       <c r="G7" s="29">
@@ -8151,10 +8136,10 @@
       <c r="H7" s="29">
         <v>1</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>8</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="29">
         <v>8</v>
       </c>
       <c r="K7" s="19">
@@ -8163,16 +8148,16 @@
       <c r="L7" s="29">
         <v>128</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M7" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="31">
         <v>-6.25E-2</v>
       </c>
-      <c r="O7" s="32">
-        <v>1</v>
-      </c>
-      <c r="P7" s="44">
+      <c r="O7" s="29">
+        <v>1</v>
+      </c>
+      <c r="P7" s="39">
         <v>256</v>
       </c>
     </row>
@@ -8182,13 +8167,13 @@
       <c r="C8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="36">
         <v>256</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="29">
         <v>64</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="31">
         <v>3.90625E-3</v>
       </c>
       <c r="G8" s="29">
@@ -8197,10 +8182,10 @@
       <c r="H8" s="29">
         <v>2.4</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="29">
         <v>256</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="29">
         <v>32</v>
       </c>
       <c r="K8" s="29">
@@ -8215,10 +8200,10 @@
       <c r="N8" s="13">
         <v>-3.90625E-3</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="29">
         <v>32</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="39">
         <v>8</v>
       </c>
     </row>
@@ -8232,16 +8217,16 @@
       <c r="C9" s="21">
         <v>1</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="36">
         <v>16</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="29">
         <v>4</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="29">
         <v>4</v>
       </c>
       <c r="H9" s="29">
@@ -8256,7 +8241,7 @@
       <c r="K9" s="19">
         <v>2.4</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="31">
         <v>3.125E-2</v>
       </c>
       <c r="M9" s="32">
@@ -8265,10 +8250,10 @@
       <c r="N9" s="13">
         <v>3.125E-2</v>
       </c>
-      <c r="O9" s="32">
+      <c r="O9" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="P9" s="43">
+      <c r="P9" s="39">
         <v>1</v>
       </c>
     </row>
@@ -8277,43 +8262,43 @@
       <c r="C10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="36">
         <v>2</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="29">
         <v>8</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="31">
         <v>7.8125E-3</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="31">
         <v>6.25E-2</v>
       </c>
       <c r="H10" s="19">
         <v>2.4</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>2</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="29">
         <v>2</v>
       </c>
       <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="31">
         <v>0.125</v>
       </c>
       <c r="M10" s="32">
         <v>3.90625E-3</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="O10" s="29">
+      <c r="O10" s="31">
         <v>3.90625E-3</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8325,16 +8310,16 @@
       <c r="C11" s="22">
         <v>1</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="36">
         <v>64</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="29">
         <v>8</v>
       </c>
       <c r="F11" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="29">
         <v>2</v>
       </c>
       <c r="H11" s="19">
@@ -8355,13 +8340,13 @@
       <c r="M11" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="29">
         <v>-1</v>
       </c>
-      <c r="O11" s="32">
+      <c r="O11" s="13">
         <v>0.125</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="39">
         <v>64</v>
       </c>
     </row>
@@ -8371,31 +8356,31 @@
       <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="36">
         <v>1024</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="29">
         <v>4</v>
       </c>
-      <c r="F12" s="13">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="F12" s="29">
+        <v>1</v>
+      </c>
+      <c r="G12" s="29">
         <v>1024</v>
       </c>
       <c r="H12" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="29">
         <v>4</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="29">
         <v>2</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="19">
         <v>0.2</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="13">
         <v>9.765625E-4</v>
       </c>
       <c r="M12" s="32">
@@ -8404,10 +8389,10 @@
       <c r="N12" s="13">
         <v>0.125</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="13">
         <v>1.953125E-3</v>
       </c>
-      <c r="P12" s="43">
+      <c r="P12" s="39">
         <v>32</v>
       </c>
     </row>
@@ -8421,25 +8406,25 @@
       <c r="C13" s="21">
         <v>1</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="36">
         <v>32</v>
       </c>
       <c r="E13" s="29">
         <v>128</v>
       </c>
-      <c r="F13" s="31">
-        <v>1</v>
-      </c>
-      <c r="G13" s="30">
+      <c r="F13" s="29">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
         <v>3.90625E-3</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="29">
         <v>1</v>
       </c>
       <c r="I13" s="29">
         <v>8</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="29">
         <v>32</v>
       </c>
       <c r="K13" s="19">
@@ -8451,13 +8436,13 @@
       <c r="M13" s="13">
         <v>1.5625E-2</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="29">
         <v>-2</v>
       </c>
-      <c r="O13" s="32">
+      <c r="O13" s="29">
         <v>1024</v>
       </c>
-      <c r="P13" s="45">
+      <c r="P13" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8466,43 +8451,43 @@
       <c r="C14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="36">
         <v>0</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="29">
         <v>16</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="19">
         <v>0.5</v>
       </c>
       <c r="H14" s="29">
         <v>3</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="30">
         <v>0.25</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="29">
         <v>4</v>
       </c>
       <c r="K14" s="19">
         <v>2.8</v>
       </c>
-      <c r="L14" s="32">
+      <c r="L14" s="29">
         <v>128</v>
       </c>
       <c r="M14" s="31">
         <v>3.90625E-3</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="31">
         <v>-1.953125E-3</v>
       </c>
-      <c r="O14" s="29">
+      <c r="O14" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="39">
         <v>32</v>
       </c>
     </row>
@@ -8514,13 +8499,13 @@
       <c r="C15" s="22">
         <v>1</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="36">
         <v>256</v>
       </c>
       <c r="E15" s="29">
         <v>32</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="13">
         <v>0.125</v>
       </c>
       <c r="G15" s="29">
@@ -8532,25 +8517,25 @@
       <c r="I15" s="29">
         <v>1024</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="31">
         <v>6.25E-2</v>
       </c>
       <c r="K15" s="19">
         <v>3</v>
       </c>
-      <c r="L15" s="32">
+      <c r="L15" s="29">
         <v>4</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="N15" s="30">
+      <c r="N15" s="29">
         <v>-16</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="29">
         <v>32</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8560,7 +8545,7 @@
       <c r="C16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="35">
         <v>1.5625E-2</v>
       </c>
       <c r="E16" s="29">
@@ -8569,16 +8554,16 @@
       <c r="F16" s="29">
         <v>1024</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="29">
         <v>16</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="29">
         <v>3</v>
       </c>
       <c r="I16" s="29">
         <v>512</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="29">
         <v>1</v>
       </c>
       <c r="K16" s="29">
@@ -8587,16 +8572,16 @@
       <c r="L16" s="29">
         <v>512</v>
       </c>
-      <c r="M16" s="32">
-        <v>1</v>
-      </c>
-      <c r="N16" s="19">
+      <c r="M16" s="29">
+        <v>1</v>
+      </c>
+      <c r="N16" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="O16" s="30">
+      <c r="O16" s="31">
         <v>3.90625E-3</v>
       </c>
-      <c r="P16" s="45">
+      <c r="P16" s="38">
         <v>1.5625E-2</v>
       </c>
     </row>
@@ -8610,13 +8595,13 @@
       <c r="C17" s="22">
         <v>1</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="36">
         <v>64</v>
       </c>
       <c r="E17" s="29">
         <v>4</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="31">
         <v>6.25E-2</v>
       </c>
       <c r="G17" s="29">
@@ -8628,7 +8613,7 @@
       <c r="I17" s="29">
         <v>8</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="29">
         <v>16</v>
       </c>
       <c r="K17" s="29">
@@ -8637,7 +8622,7 @@
       <c r="L17" s="29">
         <v>256</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="31">
         <v>7.8125E-3</v>
       </c>
       <c r="N17" s="19">
@@ -8646,7 +8631,7 @@
       <c r="O17" s="29">
         <v>2</v>
       </c>
-      <c r="P17" s="45">
+      <c r="P17" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8655,13 +8640,13 @@
       <c r="C18" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="40">
-        <v>1</v>
-      </c>
-      <c r="E18" s="32">
+      <c r="D18" s="36">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
         <v>4</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="30">
         <v>1.5625E-2</v>
       </c>
       <c r="G18" s="29">
@@ -8673,7 +8658,7 @@
       <c r="I18" s="29">
         <v>16</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="29">
         <v>2</v>
       </c>
       <c r="K18" s="29">
@@ -8682,16 +8667,16 @@
       <c r="L18" s="29">
         <v>512</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="N18" s="19">
-        <v>1</v>
-      </c>
-      <c r="O18" s="29">
+      <c r="N18" s="29">
+        <v>1</v>
+      </c>
+      <c r="O18" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8703,25 +8688,25 @@
       <c r="C19" s="22">
         <v>1</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="36">
         <v>4</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="29">
         <v>8</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="31">
         <v>7.8125E-3</v>
       </c>
       <c r="G19" s="29">
         <v>0.5</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="29">
         <v>3</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="29">
         <v>16</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="29">
         <v>16</v>
       </c>
       <c r="K19" s="19">
@@ -8736,10 +8721,10 @@
       <c r="N19" s="13">
         <v>-0.125</v>
       </c>
-      <c r="O19" s="29">
+      <c r="O19" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="39">
         <v>16</v>
       </c>
     </row>
@@ -8749,43 +8734,43 @@
       <c r="C20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="37">
         <v>2</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="42">
         <v>4</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="60">
         <v>1.5625E-2</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="40">
         <v>0.25</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="42">
         <v>2</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="42">
         <v>8</v>
       </c>
-      <c r="J20" s="35">
+      <c r="J20" s="42">
         <v>4</v>
       </c>
-      <c r="K20" s="48">
+      <c r="K20" s="41">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L20" s="49">
+      <c r="L20" s="42">
         <v>512</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M20" s="60">
         <v>1.5625E-2</v>
       </c>
       <c r="N20" s="14">
         <v>-9.765625E-4</v>
       </c>
-      <c r="O20" s="46">
+      <c r="O20" s="14">
         <v>0.125</v>
       </c>
-      <c r="P20" s="51">
+      <c r="P20" s="53">
         <v>4</v>
       </c>
     </row>
@@ -9046,8 +9031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9055,15 +9040,14 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -9071,61 +9055,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="57"/>
+      <c r="F3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="62" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="62" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="62" t="s">
+      <c r="K3" s="57"/>
+      <c r="L3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="63"/>
-      <c r="N3" s="62" t="s">
+      <c r="M3" s="57"/>
+      <c r="N3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="62" t="s">
+      <c r="O3" s="57"/>
+      <c r="P3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="62" t="s">
+      <c r="Q3" s="57"/>
+      <c r="R3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="64"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -9262,7 +9246,7 @@
       <c r="G6" s="29">
         <v>1024.001</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <v>32</v>
       </c>
       <c r="I6" s="29">
@@ -9307,7 +9291,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>8</v>
       </c>
       <c r="E7" s="29">
@@ -9319,7 +9303,7 @@
       <c r="G7" s="29">
         <v>1024.001</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="29">
         <v>1</v>
       </c>
       <c r="I7" s="29">
@@ -9331,7 +9315,7 @@
       <c r="K7" s="29">
         <v>1024.001</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="30">
         <v>0.25</v>
       </c>
       <c r="M7" s="29">
@@ -9362,7 +9346,7 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>8</v>
       </c>
       <c r="E8" s="29">
@@ -9386,13 +9370,13 @@
       <c r="K8" s="29">
         <v>1024.001</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="31">
         <v>1.5625E-2</v>
       </c>
       <c r="M8" s="29">
         <v>1024.001</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="29">
         <v>-1024</v>
       </c>
       <c r="O8" s="29">
@@ -9424,31 +9408,31 @@
       <c r="D9" s="30">
         <v>0.8</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="29">
         <v>1</v>
       </c>
       <c r="F9" s="19">
         <v>0.5</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="29">
         <v>1</v>
       </c>
       <c r="H9" s="30">
         <v>0.9</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="29">
         <v>1</v>
       </c>
       <c r="J9" s="30">
         <v>0.3</v>
       </c>
-      <c r="K9" s="13">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
+      <c r="K9" s="29">
+        <v>1</v>
+      </c>
+      <c r="L9" s="31">
         <v>1E-4</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="29">
         <v>1</v>
       </c>
       <c r="N9" s="19">
@@ -9460,13 +9444,13 @@
       <c r="P9" s="30">
         <v>0.8</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="29">
         <v>1</v>
       </c>
       <c r="R9" s="19">
         <v>0.1</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="29">
         <v>1</v>
       </c>
     </row>
@@ -9478,31 +9462,31 @@
       <c r="D10" s="30">
         <v>0.8</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="29">
         <v>1</v>
       </c>
       <c r="F10" s="19">
         <v>0.9</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="29">
         <v>1</v>
       </c>
       <c r="H10" s="30">
         <v>0.8</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="29">
         <v>1</v>
       </c>
       <c r="J10" s="19">
         <v>0.3</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="29">
         <v>1</v>
       </c>
       <c r="L10" s="30">
         <v>0.3</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="29">
         <v>1</v>
       </c>
       <c r="N10" s="30">
@@ -9514,13 +9498,13 @@
       <c r="P10" s="30">
         <v>0.8</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="29">
         <v>1</v>
       </c>
       <c r="R10" s="30">
         <v>0.5</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="29">
         <v>1</v>
       </c>
     </row>
@@ -9535,31 +9519,31 @@
       <c r="D11" s="30">
         <v>0.9</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="29">
         <v>1</v>
       </c>
       <c r="F11" s="30">
         <v>0.3</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="29">
         <v>1</v>
       </c>
       <c r="H11" s="30">
         <v>0.9</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="29">
         <v>1</v>
       </c>
       <c r="J11" s="30">
         <v>0.8</v>
       </c>
-      <c r="K11" s="13">
-        <v>1</v>
-      </c>
-      <c r="L11" s="30">
+      <c r="K11" s="29">
+        <v>1</v>
+      </c>
+      <c r="L11" s="29">
         <v>0.999</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="29">
         <v>1</v>
       </c>
       <c r="N11" s="19">
@@ -9571,13 +9555,13 @@
       <c r="P11" s="30">
         <v>0.9</v>
       </c>
-      <c r="Q11" s="13">
-        <v>1</v>
-      </c>
-      <c r="R11" s="19">
+      <c r="Q11" s="29">
+        <v>1</v>
+      </c>
+      <c r="R11" s="30">
         <v>0.99</v>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="29">
         <v>1</v>
       </c>
     </row>
@@ -9590,31 +9574,31 @@
       <c r="D12" s="30">
         <v>0.99</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="29">
         <v>1</v>
       </c>
       <c r="F12" s="30">
         <v>0.4</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="29">
         <v>1</v>
       </c>
       <c r="H12" s="30">
         <v>0.99</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="29">
         <v>1</v>
       </c>
       <c r="J12" s="19">
         <v>0.4</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="29">
         <v>1</v>
       </c>
       <c r="L12" s="30">
         <v>0.2</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="29">
         <v>1</v>
       </c>
       <c r="N12" s="19">
@@ -9626,13 +9610,13 @@
       <c r="P12" s="30">
         <v>0.9</v>
       </c>
-      <c r="Q12" s="13">
-        <v>1</v>
-      </c>
-      <c r="R12" s="19">
+      <c r="Q12" s="29">
+        <v>1</v>
+      </c>
+      <c r="R12" s="30">
         <v>0.99</v>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="29">
         <v>1</v>
       </c>
     </row>
@@ -9646,22 +9630,22 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="29">
         <v>8</v>
       </c>
       <c r="E13" s="29">
         <v>16.0009765625</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="13">
         <v>2.9296875E-3</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="29">
         <v>8</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="29">
         <v>512.0009765625</v>
       </c>
       <c r="J13" s="13">
@@ -9670,28 +9654,28 @@
       <c r="K13" s="29">
         <v>4.0009765625</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="29">
         <v>64.0009765625</v>
       </c>
       <c r="N13" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="29">
         <v>64.0009765625</v>
       </c>
       <c r="P13" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="Q13" s="31">
+      <c r="Q13" s="29">
         <v>16.0009765625</v>
       </c>
       <c r="R13" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="29">
         <v>4.0009765625</v>
       </c>
     </row>
@@ -9700,7 +9684,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="29">
         <v>8</v>
       </c>
       <c r="E14" s="29">
@@ -9709,10 +9693,10 @@
       <c r="F14" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="29">
         <v>256.0009765625</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="29">
         <v>1</v>
       </c>
       <c r="I14" s="29">
@@ -9739,13 +9723,13 @@
       <c r="P14" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="Q14" s="31">
+      <c r="Q14" s="29">
         <v>16.0009765625</v>
       </c>
       <c r="R14" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="29">
         <v>2.0009765625</v>
       </c>
     </row>
@@ -9760,7 +9744,7 @@
       <c r="D15" s="29">
         <v>128</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="29">
         <v>1024.0009765625</v>
       </c>
       <c r="F15" s="29">
@@ -9769,16 +9753,16 @@
       <c r="G15" s="29">
         <v>1.0009765625</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="31">
         <v>1.66015625E-2</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="29">
         <v>16.0009765625</v>
       </c>
       <c r="L15" s="29">
@@ -9787,19 +9771,19 @@
       <c r="M15" s="29">
         <v>256.0009765625</v>
       </c>
-      <c r="N15" s="29">
+      <c r="N15" s="13">
         <v>3.125E-2</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="29">
         <v>128.0009765625</v>
       </c>
-      <c r="P15" s="29">
+      <c r="P15" s="13">
         <v>3.125E-2</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="Q15" s="13">
         <v>0.1259765625</v>
       </c>
-      <c r="R15" s="29">
+      <c r="R15" s="13">
         <v>0.25</v>
       </c>
       <c r="S15" s="13">
@@ -9815,16 +9799,16 @@
       <c r="D16" s="29">
         <v>64</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="13">
         <v>8.7890625E-3</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="31">
         <v>1.5625E-2</v>
       </c>
       <c r="G16" s="19">
         <v>0.5009765625</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="29">
         <v>128</v>
       </c>
       <c r="I16" s="29">
@@ -9833,10 +9817,10 @@
       <c r="J16" s="29">
         <v>512</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="13">
         <v>6.34765625E-2</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="29">
         <v>8</v>
       </c>
       <c r="M16" s="29">
@@ -9845,19 +9829,19 @@
       <c r="N16" s="29">
         <v>4</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="29">
         <v>1024.0009765625</v>
       </c>
-      <c r="P16" s="13">
+      <c r="P16" s="29">
         <v>256</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="Q16" s="29">
         <v>16.0009765625</v>
       </c>
-      <c r="R16" s="29">
+      <c r="R16" s="13">
         <v>7.8125E-3</v>
       </c>
-      <c r="S16" s="13">
+      <c r="S16" s="29">
         <v>8.0009765625</v>
       </c>
     </row>
@@ -9889,22 +9873,22 @@
       <c r="I17" s="29">
         <v>1024.0009765625</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="30">
         <v>0.5</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="29">
         <v>256.0009765625</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="29">
         <v>128</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="29">
         <v>1024.0009765625</v>
       </c>
-      <c r="N17" s="29">
+      <c r="N17" s="13">
         <v>-0.25</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="29">
         <v>2.0009765625</v>
       </c>
       <c r="P17" s="31">
@@ -9925,19 +9909,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="13">
         <v>9.765625E-4</v>
       </c>
       <c r="E18" s="29">
         <v>16.0009765625</v>
       </c>
-      <c r="F18" s="31">
-        <v>1</v>
-      </c>
-      <c r="G18" s="19">
+      <c r="F18" s="29">
+        <v>1</v>
+      </c>
+      <c r="G18" s="29">
         <v>64.0009765625</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="29">
         <v>16</v>
       </c>
       <c r="I18" s="29">
@@ -9949,16 +9933,16 @@
       <c r="K18" s="29">
         <v>64.0009765625</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="30">
         <v>0.5</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="29">
         <v>2.0009765625</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="29">
         <v>8</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="29">
         <v>32.0009765625</v>
       </c>
       <c r="P18" s="13">
@@ -9982,10 +9966,10 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="13">
         <v>1.953125E-3</v>
       </c>
       <c r="F19" s="30">
@@ -10003,7 +9987,7 @@
       <c r="J19" s="31">
         <v>9.765625E-4</v>
       </c>
-      <c r="K19" s="29">
+      <c r="K19" s="13">
         <v>2.9296875E-3</v>
       </c>
       <c r="L19" s="31">
@@ -10012,13 +9996,13 @@
       <c r="M19" s="29">
         <v>128.0009765625</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="29">
         <v>-256</v>
       </c>
-      <c r="O19" s="29">
+      <c r="O19" s="13">
         <v>4.8828125E-3</v>
       </c>
-      <c r="P19" s="31">
+      <c r="P19" s="29">
         <v>2</v>
       </c>
       <c r="Q19" s="29">
@@ -10027,7 +10011,7 @@
       <c r="R19" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="S19" s="13">
+      <c r="S19" s="29">
         <v>16.0009765625</v>
       </c>
     </row>
@@ -10037,7 +10021,7 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="29">
         <v>1</v>
       </c>
       <c r="E20" s="29">
@@ -10052,13 +10036,13 @@
       <c r="H20" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="29">
         <v>4.0009765625</v>
       </c>
       <c r="J20" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="13">
         <v>0.2509765625</v>
       </c>
       <c r="L20" s="31">
@@ -10070,19 +10054,19 @@
       <c r="N20" s="29">
         <v>-1</v>
       </c>
-      <c r="O20" s="29">
+      <c r="O20" s="30">
         <v>-0.2490234375</v>
       </c>
       <c r="P20" s="13">
         <v>7.8125E-3</v>
       </c>
-      <c r="Q20" s="13">
+      <c r="Q20" s="29">
         <v>16.0009765625</v>
       </c>
-      <c r="R20" s="31">
+      <c r="R20" s="30">
         <v>0.25</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="29">
         <v>8.0009765625</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started datasets analysis updating excel files
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_01_hold2.xlsx
+++ b/results_analysis/spark_cervicalCancer_01_hold2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45887021-C104-46C6-A4F8-21C6247C48D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5801E-3934-4F1D-9D98-370DF13A0A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
-    <sheet name="acc_median" sheetId="7" r:id="rId2"/>
-    <sheet name="acc_best" sheetId="11" r:id="rId3"/>
+    <sheet name="acc_best" sheetId="11" r:id="rId1"/>
+    <sheet name="acc_mean" sheetId="1" r:id="rId2"/>
+    <sheet name="acc_median" sheetId="7" r:id="rId3"/>
     <sheet name="nprot_best" sheetId="3" r:id="rId4"/>
     <sheet name="nprot_mean" sheetId="8" r:id="rId5"/>
     <sheet name="K_best" sheetId="9" r:id="rId6"/>
@@ -677,6 +677,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,9 +696,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -977,10 +977,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4279F1E-80F5-41C1-B97A-BFBE1F0D2B01}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -999,19 +999,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1060,28 +1060,28 @@
         <v>1</v>
       </c>
       <c r="D5" s="44">
-        <v>0.42578397212543601</v>
+        <v>0.494773519163763</v>
       </c>
       <c r="E5" s="12">
-        <v>0.36689895470383299</v>
+        <v>0.41986062717770001</v>
       </c>
       <c r="F5" s="12">
-        <v>0.38135888501742199</v>
+        <v>0.42857142857142899</v>
       </c>
       <c r="G5" s="12">
-        <v>0.38048780487804901</v>
+        <v>0.41289198606271799</v>
       </c>
       <c r="H5" s="12">
-        <v>0.39843205574912899</v>
+        <v>0.44076655052264802</v>
       </c>
       <c r="I5" s="12">
-        <v>0.44965156794425098</v>
+        <v>0.48432055749128899</v>
       </c>
       <c r="J5" s="12">
-        <v>0.36411149825784</v>
+        <v>0.45644599303135902</v>
       </c>
       <c r="K5" s="45">
-        <v>0.37979094076655101</v>
+        <v>0.43031358885017401</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1090,28 +1090,28 @@
         <v>12</v>
       </c>
       <c r="D6" s="46">
-        <v>0.39686411149825801</v>
+        <v>0.454703832752613</v>
       </c>
       <c r="E6" s="13">
-        <v>0.39076655052264803</v>
+        <v>0.46341463414634199</v>
       </c>
       <c r="F6" s="13">
-        <v>0.406794425087108</v>
+        <v>0.45644599303135902</v>
       </c>
       <c r="G6" s="13">
-        <v>0.42038327526132402</v>
+        <v>0.48780487804878098</v>
       </c>
       <c r="H6" s="13">
-        <v>0.41707317073170702</v>
+        <v>0.46515679442508701</v>
       </c>
       <c r="I6" s="13">
-        <v>0.435017421602787</v>
+        <v>0.49651567944250902</v>
       </c>
       <c r="J6" s="13">
-        <v>0.37526132404181201</v>
+        <v>0.46864111498257799</v>
       </c>
       <c r="K6" s="15">
-        <v>0.41898954703832803</v>
+        <v>0.48083623693379801</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1123,28 +1123,28 @@
         <v>1</v>
       </c>
       <c r="D7" s="46">
-        <v>0.39721254355400698</v>
+        <v>0.43379790940766599</v>
       </c>
       <c r="E7" s="13">
-        <v>0.39250871080139399</v>
+        <v>0.43205574912891997</v>
       </c>
       <c r="F7" s="13">
-        <v>0.39337979094076603</v>
+        <v>0.42160278745644603</v>
       </c>
       <c r="G7" s="13">
-        <v>0.36271777003484301</v>
+        <v>0.40418118466899</v>
       </c>
       <c r="H7" s="13">
-        <v>0.34790940766550499</v>
+        <v>0.398954703832753</v>
       </c>
       <c r="I7" s="13">
-        <v>0.408188153310105</v>
+        <v>0.50174216027874596</v>
       </c>
       <c r="J7" s="13">
-        <v>0.38745644599303097</v>
+        <v>0.45644599303135902</v>
       </c>
       <c r="K7" s="15">
-        <v>0.381881533101045</v>
+        <v>0.42508710801393701</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1154,28 +1154,28 @@
         <v>12</v>
       </c>
       <c r="D8" s="47">
-        <v>0.43222996515679402</v>
+        <v>0.47212543554007003</v>
       </c>
       <c r="E8" s="14">
-        <v>0.40470383275261301</v>
+        <v>0.47386759581881499</v>
       </c>
       <c r="F8" s="14">
-        <v>0.42090592334494797</v>
+        <v>0.46689895470383302</v>
       </c>
       <c r="G8" s="14">
-        <v>0.40958188153310099</v>
+        <v>0.46515679442508701</v>
       </c>
       <c r="H8" s="14">
-        <v>0.430487804878049</v>
+        <v>0.45296167247386798</v>
       </c>
       <c r="I8" s="14">
-        <v>0.38501742160278701</v>
+        <v>0.510452961672474</v>
       </c>
       <c r="J8" s="14">
-        <v>0.41411149825783999</v>
+        <v>0.47386759581881499</v>
       </c>
       <c r="K8" s="48">
-        <v>0.40191637630662003</v>
+        <v>0.45993031358885</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1189,28 +1189,28 @@
         <v>1</v>
       </c>
       <c r="D9" s="49">
-        <v>0.39407665505226502</v>
+        <v>0.45644599303135902</v>
       </c>
       <c r="E9" s="50">
-        <v>0.39773519163763099</v>
+        <v>0.449477351916376</v>
       </c>
       <c r="F9" s="50">
-        <v>0.37282229965156799</v>
+        <v>0.45121951219512202</v>
       </c>
       <c r="G9" s="50">
-        <v>0.40975609756097597</v>
+        <v>0.46167247386759602</v>
       </c>
       <c r="H9" s="50">
-        <v>0.39285714285714302</v>
+        <v>0.41811846689895499</v>
       </c>
       <c r="I9" s="50">
-        <v>0.15331010452961699</v>
+        <v>0.257839721254355</v>
       </c>
       <c r="J9" s="50">
-        <v>0.36724738675958202</v>
+        <v>0.439024390243902</v>
       </c>
       <c r="K9" s="51">
-        <v>0.39285714285714302</v>
+        <v>0.46515679442508701</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1219,28 +1219,28 @@
         <v>12</v>
       </c>
       <c r="D10" s="46">
-        <v>0.412020905923345</v>
+        <v>0.45818815331010498</v>
       </c>
       <c r="E10" s="13">
-        <v>0.37508710801393702</v>
+        <v>0.43031358885017401</v>
       </c>
       <c r="F10" s="13">
-        <v>0.420557491289199</v>
+        <v>0.47560975609756101</v>
       </c>
       <c r="G10" s="13">
-        <v>0.406794425087108</v>
+        <v>0.49128919860627202</v>
       </c>
       <c r="H10" s="13">
-        <v>0.41184668989547002</v>
+        <v>0.49651567944250902</v>
       </c>
       <c r="I10" s="13">
-        <v>0.17020905923345001</v>
+        <v>0.257839721254355</v>
       </c>
       <c r="J10" s="13">
-        <v>0.42073170731707299</v>
+        <v>0.48083623693379801</v>
       </c>
       <c r="K10" s="15">
-        <v>0.40365853658536599</v>
+        <v>0.46515679442508701</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1252,28 +1252,28 @@
         <v>1</v>
       </c>
       <c r="D11" s="46">
-        <v>0.39494773519163801</v>
+        <v>0.44250871080139398</v>
       </c>
       <c r="E11" s="13">
-        <v>0.37317073170731702</v>
+        <v>0.43379790940766599</v>
       </c>
       <c r="F11" s="13">
-        <v>0.368118466898955</v>
+        <v>0.44076655052264802</v>
       </c>
       <c r="G11" s="13">
-        <v>0.37648083623693401</v>
+        <v>0.42160278745644603</v>
       </c>
       <c r="H11" s="13">
-        <v>0.37055749128919901</v>
+        <v>0.41463414634146301</v>
       </c>
       <c r="I11" s="13">
-        <v>0.32648083623693402</v>
+        <v>0.40069686411149802</v>
       </c>
       <c r="J11" s="13">
-        <v>0.36986062717770002</v>
+        <v>0.409407665505227</v>
       </c>
       <c r="K11" s="15">
-        <v>0.36655052264808402</v>
+        <v>0.41289198606271799</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1283,28 +1283,28 @@
         <v>12</v>
       </c>
       <c r="D12" s="47">
-        <v>0.39581881533100999</v>
+        <v>0.46864111498257799</v>
       </c>
       <c r="E12" s="14">
-        <v>0.42822299651567902</v>
+        <v>0.47560975609756101</v>
       </c>
       <c r="F12" s="14">
-        <v>0.38763066202090601</v>
+        <v>0.47909407665505199</v>
       </c>
       <c r="G12" s="14">
-        <v>0.40609756097561001</v>
+        <v>0.494773519163763</v>
       </c>
       <c r="H12" s="14">
-        <v>0.40452961672473903</v>
+        <v>0.439024390243902</v>
       </c>
       <c r="I12" s="14">
-        <v>0.32648083623693402</v>
+        <v>0.36585365853658502</v>
       </c>
       <c r="J12" s="14">
-        <v>0.40644599303135898</v>
+        <v>0.489547038327526</v>
       </c>
       <c r="K12" s="48">
-        <v>0.43519163763066199</v>
+        <v>0.52439024390243905</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1318,28 +1318,28 @@
         <v>1</v>
       </c>
       <c r="D13" s="49">
-        <v>0.395644599303136</v>
+        <v>0.444250871080139</v>
       </c>
       <c r="E13" s="50">
-        <v>0.40017421602787501</v>
+        <v>0.44599303135888502</v>
       </c>
       <c r="F13" s="50">
-        <v>0.38397212543553999</v>
+        <v>0.43205574912891997</v>
       </c>
       <c r="G13" s="50">
-        <v>0.38310104529616701</v>
+        <v>0.44773519163763098</v>
       </c>
       <c r="H13" s="50">
-        <v>0.36829268292682898</v>
+        <v>0.43379790940766599</v>
       </c>
       <c r="I13" s="50">
-        <v>0.38693379790940802</v>
+        <v>0.444250871080139</v>
       </c>
       <c r="J13" s="50">
-        <v>0.37038327526132397</v>
+        <v>0.46864111498257799</v>
       </c>
       <c r="K13" s="51">
-        <v>0.39320557491289199</v>
+        <v>0.44250871080139398</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1348,28 +1348,28 @@
         <v>12</v>
       </c>
       <c r="D14" s="46">
-        <v>0.42404181184668999</v>
+        <v>0.46167247386759602</v>
       </c>
       <c r="E14" s="13">
-        <v>0.42787456445993</v>
+        <v>0.48257839721254397</v>
       </c>
       <c r="F14" s="13">
-        <v>0.42264808362369299</v>
+        <v>0.48432055749128899</v>
       </c>
       <c r="G14" s="13">
-        <v>0.440243902439024</v>
+        <v>0.48780487804878098</v>
       </c>
       <c r="H14" s="13">
-        <v>0.42299651567944202</v>
+        <v>0.47735191637630697</v>
       </c>
       <c r="I14" s="13">
-        <v>0.40331010452961702</v>
+        <v>0.48606271777003501</v>
       </c>
       <c r="J14" s="13">
-        <v>0.40888501742160299</v>
+        <v>0.494773519163763</v>
       </c>
       <c r="K14" s="15">
-        <v>0.40923344947735202</v>
+        <v>0.46689895470383302</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1381,28 +1381,28 @@
         <v>1</v>
       </c>
       <c r="D15" s="46">
-        <v>0.34198606271776999</v>
+        <v>0.398954703832753</v>
       </c>
       <c r="E15" s="13">
-        <v>0.28432055749128898</v>
+        <v>0.454703832752613</v>
       </c>
       <c r="F15" s="13">
-        <v>0.22351916376306599</v>
+        <v>0.41637630662020902</v>
       </c>
       <c r="G15" s="13">
-        <v>0.25818815331010497</v>
+        <v>0.41637630662020902</v>
       </c>
       <c r="H15" s="13">
-        <v>0.35418118466899001</v>
+        <v>0.45296167247386798</v>
       </c>
       <c r="I15" s="13">
-        <v>0.326132404181185</v>
+        <v>0.43031358885017401</v>
       </c>
       <c r="J15" s="13">
-        <v>0.166724738675958</v>
+        <v>0.37804878048780499</v>
       </c>
       <c r="K15" s="15">
-        <v>0.21968641114982601</v>
+        <v>0.39198606271776998</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1412,28 +1412,28 @@
         <v>12</v>
       </c>
       <c r="D16" s="47">
-        <v>0.333275261324042</v>
+        <v>0.39547038327526102</v>
       </c>
       <c r="E16" s="14">
-        <v>0.22944250871080099</v>
+        <v>0.38327526132404199</v>
       </c>
       <c r="F16" s="14">
-        <v>0.247735191637631</v>
+        <v>0.348432055749129</v>
       </c>
       <c r="G16" s="14">
-        <v>0.16811846689895499</v>
+        <v>0.39198606271776998</v>
       </c>
       <c r="H16" s="14">
-        <v>0.36062717770034802</v>
+        <v>0.43379790940766599</v>
       </c>
       <c r="I16" s="14">
-        <v>0.32700348432055798</v>
+        <v>0.39198606271776998</v>
       </c>
       <c r="J16" s="14">
-        <v>0.23118466898954701</v>
+        <v>0.36411149825784</v>
       </c>
       <c r="K16" s="48">
-        <v>0.19668989547038301</v>
+        <v>0.393728222996516</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1447,28 +1447,28 @@
         <v>1</v>
       </c>
       <c r="D17" s="49">
-        <v>0.463240418118467</v>
+        <v>0.49825783972125398</v>
       </c>
       <c r="E17" s="50">
-        <v>0.46010452961672499</v>
+        <v>0.49825783972125398</v>
       </c>
       <c r="F17" s="50">
-        <v>0.40331010452961702</v>
+        <v>0.43728222996515698</v>
       </c>
       <c r="G17" s="50">
-        <v>0.43658536585365898</v>
+        <v>0.48257839721254397</v>
       </c>
       <c r="H17" s="50">
-        <v>0.42212543554006998</v>
+        <v>0.48432055749128899</v>
       </c>
       <c r="I17" s="50">
-        <v>0.36202090592334502</v>
+        <v>0.43554006968641101</v>
       </c>
       <c r="J17" s="50">
-        <v>0.36986062717770002</v>
+        <v>0.45993031358885</v>
       </c>
       <c r="K17" s="51">
-        <v>0.44529616724738702</v>
+        <v>0.50696864111498297</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1477,28 +1477,28 @@
         <v>12</v>
       </c>
       <c r="D18" s="46">
-        <v>0.48780487804878098</v>
+        <v>0.54355400696864098</v>
       </c>
       <c r="E18" s="13">
-        <v>0.49686411149825799</v>
+        <v>0.52264808362369297</v>
       </c>
       <c r="F18" s="13">
-        <v>0.44477351916376301</v>
+        <v>0.505226480836237</v>
       </c>
       <c r="G18" s="13">
-        <v>0.42508710801393701</v>
+        <v>0.47560975609756101</v>
       </c>
       <c r="H18" s="13">
-        <v>0.449477351916376</v>
+        <v>0.48432055749128899</v>
       </c>
       <c r="I18" s="13">
-        <v>0.39668989547038302</v>
+        <v>0.48606271777003501</v>
       </c>
       <c r="J18" s="13">
-        <v>0.435017421602787</v>
+        <v>0.49825783972125398</v>
       </c>
       <c r="K18" s="15">
-        <v>0.49564459930313598</v>
+        <v>0.51219512195121997</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1510,28 +1510,28 @@
         <v>1</v>
       </c>
       <c r="D19" s="46">
-        <v>0.398257839721254</v>
+        <v>0.43031358885017401</v>
       </c>
       <c r="E19" s="13">
-        <v>0.35801393728223002</v>
+        <v>0.40418118466899</v>
       </c>
       <c r="F19" s="13">
-        <v>0.38571428571428601</v>
+        <v>0.43205574912891997</v>
       </c>
       <c r="G19" s="13">
-        <v>0.37804878048780499</v>
+        <v>0.42334494773519199</v>
       </c>
       <c r="H19" s="13">
-        <v>0.37526132404181201</v>
+        <v>0.40592334494773502</v>
       </c>
       <c r="I19" s="13">
-        <v>0.37909407665505201</v>
+        <v>0.41986062717770001</v>
       </c>
       <c r="J19" s="13">
-        <v>0.38919860627177699</v>
+        <v>0.439024390243902</v>
       </c>
       <c r="K19" s="15">
-        <v>0.381184668989547</v>
+        <v>0.42857142857142899</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1541,28 +1541,28 @@
         <v>12</v>
       </c>
       <c r="D20" s="47">
-        <v>0.44477351916376301</v>
+        <v>0.48606271777003501</v>
       </c>
       <c r="E20" s="14">
-        <v>0.37682926829268298</v>
+        <v>0.46167247386759602</v>
       </c>
       <c r="F20" s="14">
-        <v>0.43083623693379802</v>
+        <v>0.46864111498257799</v>
       </c>
       <c r="G20" s="14">
-        <v>0.40209059233449501</v>
+        <v>0.47560975609756101</v>
       </c>
       <c r="H20" s="14">
-        <v>0.39947735191637601</v>
+        <v>0.449477351916376</v>
       </c>
       <c r="I20" s="14">
-        <v>0.43397212543553998</v>
+        <v>0.46515679442508701</v>
       </c>
       <c r="J20" s="14">
-        <v>0.41114982578397202</v>
+        <v>0.52264808362369297</v>
       </c>
       <c r="K20" s="48">
-        <v>0.40452961672473903</v>
+        <v>0.47909407665505199</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1920,19 +1920,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2523,19 +2523,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3111,6 +3111,934 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0.42578397212543601</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.36689895470383299</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.38135888501742199</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.38048780487804901</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.39843205574912899</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.44965156794425098</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.36411149825784</v>
+      </c>
+      <c r="K5" s="45">
+        <v>0.37979094076655101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="46">
+        <v>0.39686411149825801</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.39076655052264803</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.406794425087108</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.42038327526132402</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.41707317073170702</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0.435017421602787</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0.37526132404181201</v>
+      </c>
+      <c r="K6" s="15">
+        <v>0.41898954703832803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.39721254355400698</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.39250871080139399</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.39337979094076603</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.36271777003484301</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.34790940766550499</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.408188153310105</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.38745644599303097</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0.381881533101045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="47">
+        <v>0.43222996515679402</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.40470383275261301</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.42090592334494797</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.40958188153310099</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.430487804878049</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.38501742160278701</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.41411149825783999</v>
+      </c>
+      <c r="K8" s="48">
+        <v>0.40191637630662003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="49">
+        <v>0.39407665505226502</v>
+      </c>
+      <c r="E9" s="50">
+        <v>0.39773519163763099</v>
+      </c>
+      <c r="F9" s="50">
+        <v>0.37282229965156799</v>
+      </c>
+      <c r="G9" s="50">
+        <v>0.40975609756097597</v>
+      </c>
+      <c r="H9" s="50">
+        <v>0.39285714285714302</v>
+      </c>
+      <c r="I9" s="50">
+        <v>0.15331010452961699</v>
+      </c>
+      <c r="J9" s="50">
+        <v>0.36724738675958202</v>
+      </c>
+      <c r="K9" s="51">
+        <v>0.39285714285714302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="46">
+        <v>0.412020905923345</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.37508710801393702</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.420557491289199</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.406794425087108</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.41184668989547002</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0.17020905923345001</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0.42073170731707299</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.40365853658536599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="46">
+        <v>0.39494773519163801</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.37317073170731702</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.368118466898955</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.37648083623693401</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.37055749128919901</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0.32648083623693402</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.36986062717770002</v>
+      </c>
+      <c r="K11" s="15">
+        <v>0.36655052264808402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="47">
+        <v>0.39581881533100999</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.42822299651567902</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.38763066202090601</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.40609756097561001</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.40452961672473903</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.32648083623693402</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.40644599303135898</v>
+      </c>
+      <c r="K12" s="48">
+        <v>0.43519163763066199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="49">
+        <v>0.395644599303136</v>
+      </c>
+      <c r="E13" s="50">
+        <v>0.40017421602787501</v>
+      </c>
+      <c r="F13" s="50">
+        <v>0.38397212543553999</v>
+      </c>
+      <c r="G13" s="50">
+        <v>0.38310104529616701</v>
+      </c>
+      <c r="H13" s="50">
+        <v>0.36829268292682898</v>
+      </c>
+      <c r="I13" s="50">
+        <v>0.38693379790940802</v>
+      </c>
+      <c r="J13" s="50">
+        <v>0.37038327526132397</v>
+      </c>
+      <c r="K13" s="51">
+        <v>0.39320557491289199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="46">
+        <v>0.42404181184668999</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.42787456445993</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.42264808362369299</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.440243902439024</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.42299651567944202</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0.40331010452961702</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.40888501742160299</v>
+      </c>
+      <c r="K14" s="15">
+        <v>0.40923344947735202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="46">
+        <v>0.34198606271776999</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.28432055749128898</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0.22351916376306599</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.25818815331010497</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0.35418118466899001</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0.326132404181185</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.166724738675958</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0.21968641114982601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="47">
+        <v>0.333275261324042</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.22944250871080099</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.247735191637631</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0.16811846689895499</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.36062717770034802</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0.32700348432055798</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.23118466898954701</v>
+      </c>
+      <c r="K16" s="48">
+        <v>0.19668989547038301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="49">
+        <v>0.463240418118467</v>
+      </c>
+      <c r="E17" s="50">
+        <v>0.46010452961672499</v>
+      </c>
+      <c r="F17" s="50">
+        <v>0.40331010452961702</v>
+      </c>
+      <c r="G17" s="50">
+        <v>0.43658536585365898</v>
+      </c>
+      <c r="H17" s="50">
+        <v>0.42212543554006998</v>
+      </c>
+      <c r="I17" s="50">
+        <v>0.36202090592334502</v>
+      </c>
+      <c r="J17" s="50">
+        <v>0.36986062717770002</v>
+      </c>
+      <c r="K17" s="51">
+        <v>0.44529616724738702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="46">
+        <v>0.48780487804878098</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.49686411149825799</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0.44477351916376301</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.42508710801393701</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0.449477351916376</v>
+      </c>
+      <c r="I18" s="13">
+        <v>0.39668989547038302</v>
+      </c>
+      <c r="J18" s="13">
+        <v>0.435017421602787</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0.49564459930313598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="46">
+        <v>0.398257839721254</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.35801393728223002</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0.38571428571428601</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.37804878048780499</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0.37526132404181201</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0.37909407665505201</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0.38919860627177699</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0.381184668989547</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="47">
+        <v>0.44477351916376301</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.37682926829268298</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.43083623693379802</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.40209059233449501</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.39947735191637601</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0.43397212543553998</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.41114982578397202</v>
+      </c>
+      <c r="K20" s="48">
+        <v>0.40452961672473903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E17B74-8A06-473F-B1B4-0C752BEBC712}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -3133,19 +4061,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3701,934 +4629,6 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4279F1E-80F5-41C1-B97A-BFBE1F0D2B01}">
-  <dimension ref="A1:K53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="44">
-        <v>0.494773519163763</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0.41986062717770001</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0.42857142857142899</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0.41289198606271799</v>
-      </c>
-      <c r="H5" s="12">
-        <v>0.44076655052264802</v>
-      </c>
-      <c r="I5" s="12">
-        <v>0.48432055749128899</v>
-      </c>
-      <c r="J5" s="12">
-        <v>0.45644599303135902</v>
-      </c>
-      <c r="K5" s="45">
-        <v>0.43031358885017401</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="46">
-        <v>0.454703832752613</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.46341463414634199</v>
-      </c>
-      <c r="F6" s="13">
-        <v>0.45644599303135902</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.48780487804878098</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0.46515679442508701</v>
-      </c>
-      <c r="I6" s="13">
-        <v>0.49651567944250902</v>
-      </c>
-      <c r="J6" s="13">
-        <v>0.46864111498257799</v>
-      </c>
-      <c r="K6" s="15">
-        <v>0.48083623693379801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="46">
-        <v>0.43379790940766599</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.43205574912891997</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.42160278745644603</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.40418118466899</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0.398954703832753</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.50174216027874596</v>
-      </c>
-      <c r="J7" s="13">
-        <v>0.45644599303135902</v>
-      </c>
-      <c r="K7" s="15">
-        <v>0.42508710801393701</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="47">
-        <v>0.47212543554007003</v>
-      </c>
-      <c r="E8" s="14">
-        <v>0.47386759581881499</v>
-      </c>
-      <c r="F8" s="14">
-        <v>0.46689895470383302</v>
-      </c>
-      <c r="G8" s="14">
-        <v>0.46515679442508701</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0.45296167247386798</v>
-      </c>
-      <c r="I8" s="14">
-        <v>0.510452961672474</v>
-      </c>
-      <c r="J8" s="14">
-        <v>0.47386759581881499</v>
-      </c>
-      <c r="K8" s="48">
-        <v>0.45993031358885</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="49">
-        <v>0.45644599303135902</v>
-      </c>
-      <c r="E9" s="50">
-        <v>0.449477351916376</v>
-      </c>
-      <c r="F9" s="50">
-        <v>0.45121951219512202</v>
-      </c>
-      <c r="G9" s="50">
-        <v>0.46167247386759602</v>
-      </c>
-      <c r="H9" s="50">
-        <v>0.41811846689895499</v>
-      </c>
-      <c r="I9" s="50">
-        <v>0.257839721254355</v>
-      </c>
-      <c r="J9" s="50">
-        <v>0.439024390243902</v>
-      </c>
-      <c r="K9" s="51">
-        <v>0.46515679442508701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="46">
-        <v>0.45818815331010498</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.43031358885017401</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0.47560975609756101</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.49128919860627202</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0.49651567944250902</v>
-      </c>
-      <c r="I10" s="13">
-        <v>0.257839721254355</v>
-      </c>
-      <c r="J10" s="13">
-        <v>0.48083623693379801</v>
-      </c>
-      <c r="K10" s="15">
-        <v>0.46515679442508701</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="46">
-        <v>0.44250871080139398</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.43379790940766599</v>
-      </c>
-      <c r="F11" s="13">
-        <v>0.44076655052264802</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.42160278745644603</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0.41463414634146301</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0.40069686411149802</v>
-      </c>
-      <c r="J11" s="13">
-        <v>0.409407665505227</v>
-      </c>
-      <c r="K11" s="15">
-        <v>0.41289198606271799</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="47">
-        <v>0.46864111498257799</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0.47560975609756101</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0.47909407665505199</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0.494773519163763</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0.439024390243902</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0.36585365853658502</v>
-      </c>
-      <c r="J12" s="14">
-        <v>0.489547038327526</v>
-      </c>
-      <c r="K12" s="48">
-        <v>0.52439024390243905</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="49">
-        <v>0.444250871080139</v>
-      </c>
-      <c r="E13" s="50">
-        <v>0.44599303135888502</v>
-      </c>
-      <c r="F13" s="50">
-        <v>0.43205574912891997</v>
-      </c>
-      <c r="G13" s="50">
-        <v>0.44773519163763098</v>
-      </c>
-      <c r="H13" s="50">
-        <v>0.43379790940766599</v>
-      </c>
-      <c r="I13" s="50">
-        <v>0.444250871080139</v>
-      </c>
-      <c r="J13" s="50">
-        <v>0.46864111498257799</v>
-      </c>
-      <c r="K13" s="51">
-        <v>0.44250871080139398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="46">
-        <v>0.46167247386759602</v>
-      </c>
-      <c r="E14" s="13">
-        <v>0.48257839721254397</v>
-      </c>
-      <c r="F14" s="13">
-        <v>0.48432055749128899</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.48780487804878098</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0.47735191637630697</v>
-      </c>
-      <c r="I14" s="13">
-        <v>0.48606271777003501</v>
-      </c>
-      <c r="J14" s="13">
-        <v>0.494773519163763</v>
-      </c>
-      <c r="K14" s="15">
-        <v>0.46689895470383302</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="46">
-        <v>0.398954703832753</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0.454703832752613</v>
-      </c>
-      <c r="F15" s="13">
-        <v>0.41637630662020902</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.41637630662020902</v>
-      </c>
-      <c r="H15" s="13">
-        <v>0.45296167247386798</v>
-      </c>
-      <c r="I15" s="13">
-        <v>0.43031358885017401</v>
-      </c>
-      <c r="J15" s="13">
-        <v>0.37804878048780499</v>
-      </c>
-      <c r="K15" s="15">
-        <v>0.39198606271776998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="47">
-        <v>0.39547038327526102</v>
-      </c>
-      <c r="E16" s="14">
-        <v>0.38327526132404199</v>
-      </c>
-      <c r="F16" s="14">
-        <v>0.348432055749129</v>
-      </c>
-      <c r="G16" s="14">
-        <v>0.39198606271776998</v>
-      </c>
-      <c r="H16" s="14">
-        <v>0.43379790940766599</v>
-      </c>
-      <c r="I16" s="14">
-        <v>0.39198606271776998</v>
-      </c>
-      <c r="J16" s="14">
-        <v>0.36411149825784</v>
-      </c>
-      <c r="K16" s="48">
-        <v>0.393728222996516</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="49">
-        <v>0.49825783972125398</v>
-      </c>
-      <c r="E17" s="50">
-        <v>0.49825783972125398</v>
-      </c>
-      <c r="F17" s="50">
-        <v>0.43728222996515698</v>
-      </c>
-      <c r="G17" s="50">
-        <v>0.48257839721254397</v>
-      </c>
-      <c r="H17" s="50">
-        <v>0.48432055749128899</v>
-      </c>
-      <c r="I17" s="50">
-        <v>0.43554006968641101</v>
-      </c>
-      <c r="J17" s="50">
-        <v>0.45993031358885</v>
-      </c>
-      <c r="K17" s="51">
-        <v>0.50696864111498297</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="46">
-        <v>0.54355400696864098</v>
-      </c>
-      <c r="E18" s="13">
-        <v>0.52264808362369297</v>
-      </c>
-      <c r="F18" s="13">
-        <v>0.505226480836237</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.47560975609756101</v>
-      </c>
-      <c r="H18" s="13">
-        <v>0.48432055749128899</v>
-      </c>
-      <c r="I18" s="13">
-        <v>0.48606271777003501</v>
-      </c>
-      <c r="J18" s="13">
-        <v>0.49825783972125398</v>
-      </c>
-      <c r="K18" s="15">
-        <v>0.51219512195121997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="46">
-        <v>0.43031358885017401</v>
-      </c>
-      <c r="E19" s="13">
-        <v>0.40418118466899</v>
-      </c>
-      <c r="F19" s="13">
-        <v>0.43205574912891997</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0.42334494773519199</v>
-      </c>
-      <c r="H19" s="13">
-        <v>0.40592334494773502</v>
-      </c>
-      <c r="I19" s="13">
-        <v>0.41986062717770001</v>
-      </c>
-      <c r="J19" s="13">
-        <v>0.439024390243902</v>
-      </c>
-      <c r="K19" s="15">
-        <v>0.42857142857142899</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="47">
-        <v>0.48606271777003501</v>
-      </c>
-      <c r="E20" s="14">
-        <v>0.46167247386759602</v>
-      </c>
-      <c r="F20" s="14">
-        <v>0.46864111498257799</v>
-      </c>
-      <c r="G20" s="14">
-        <v>0.47560975609756101</v>
-      </c>
-      <c r="H20" s="14">
-        <v>0.449477351916376</v>
-      </c>
-      <c r="I20" s="14">
-        <v>0.46515679442508701</v>
-      </c>
-      <c r="J20" s="14">
-        <v>0.52264808362369297</v>
-      </c>
-      <c r="K20" s="48">
-        <v>0.47909407665505199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
@@ -4813,7 +4813,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,19 +4831,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5601,19 +5601,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6371,19 +6371,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7141,19 +7141,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7917,24 +7917,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7944,29 +7944,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="57"/>
-      <c r="M3" s="56" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="57"/>
-      <c r="O3" s="56" t="s">
+      <c r="N3" s="58"/>
+      <c r="O3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="58"/>
+      <c r="P3" s="59"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -8740,7 +8740,7 @@
       <c r="E20" s="42">
         <v>4</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="54">
         <v>1.5625E-2</v>
       </c>
       <c r="G20" s="40">
@@ -8761,7 +8761,7 @@
       <c r="L20" s="42">
         <v>512</v>
       </c>
-      <c r="M20" s="60">
+      <c r="M20" s="54">
         <v>1.5625E-2</v>
       </c>
       <c r="N20" s="14">
@@ -9031,7 +9031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
@@ -9055,61 +9055,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="56" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="56" t="s">
+      <c r="G3" s="58"/>
+      <c r="H3" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="56" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="56" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="57"/>
-      <c r="N3" s="56" t="s">
+      <c r="M3" s="58"/>
+      <c r="N3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="56" t="s">
+      <c r="O3" s="58"/>
+      <c r="P3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="56" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="58"/>
+      <c r="S3" s="59"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">

</xml_diff>